<commit_message>
Training and testing the models with the new test
</commit_message>
<xml_diff>
--- a/5-2 GHz Analysis/tables/models_metrics_in_test_set.xlsx
+++ b/5-2 GHz Analysis/tables/models_metrics_in_test_set.xlsx
@@ -462,13 +462,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4.03237849227961</v>
+        <v>3.335376396475537</v>
       </c>
       <c r="C2" t="n">
-        <v>3.802857628598876</v>
+        <v>3.179886475244781</v>
       </c>
       <c r="D2" t="n">
-        <v>0.4327880358721218</v>
+        <v>0.6645808329799155</v>
       </c>
     </row>
     <row r="3">
@@ -478,13 +478,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>7.724258324698019</v>
+        <v>4.559463922686821</v>
       </c>
       <c r="C3" t="n">
-        <v>7.266666666666666</v>
+        <v>4.090476190476191</v>
       </c>
       <c r="D3" t="n">
-        <v>-1.081308139534883</v>
+        <v>0.3732046855593157</v>
       </c>
     </row>
     <row r="4">
@@ -494,13 +494,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5.346469423059696</v>
+        <v>4.191087595728871</v>
       </c>
       <c r="C4" t="n">
-        <v>4.604984326373213</v>
+        <v>3.518779342723005</v>
       </c>
       <c r="D4" t="n">
-        <v>0.00285807121933912</v>
+        <v>0.4703955205505806</v>
       </c>
     </row>
     <row r="5">
@@ -510,13 +510,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3.057839183113793</v>
+        <v>1.888439805963124</v>
       </c>
       <c r="C5" t="n">
-        <v>2.796540429704236</v>
+        <v>1.55714761061008</v>
       </c>
       <c r="D5" t="n">
-        <v>0.6738239371004875</v>
+        <v>0.8924762341483605</v>
       </c>
     </row>
     <row r="6">
@@ -526,13 +526,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3.137746040682285</v>
+        <v>2.596390190944105</v>
       </c>
       <c r="C6" t="n">
-        <v>2.967863609947874</v>
+        <v>2.426800380288052</v>
       </c>
       <c r="D6" t="n">
-        <v>0.6565540622389292</v>
+        <v>0.7967464716493238</v>
       </c>
     </row>
   </sheetData>

</xml_diff>